<commit_message>
Continued on and on and on with writing amazing stuff! Also fixed some errors in the evaluation
</commit_message>
<xml_diff>
--- a/ausarbeitung/datensatz1.xlsx
+++ b/ausarbeitung/datensatz1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\post_\Documents\Uni\Masterarbeit\waldemar\ausarbeitung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A55716-28B1-42CF-BDEF-161D424E2CB2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBB85F-E5EE-464D-8FFA-1634002EEC00}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6652" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6676" uniqueCount="543">
   <si>
     <t>CASE</t>
   </si>
@@ -1663,6 +1663,39 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Median kinderlose</t>
+  </si>
+  <si>
+    <t>Median Eltern</t>
+  </si>
+  <si>
+    <t>gemeinsam</t>
+  </si>
+  <si>
+    <t>allein</t>
+  </si>
+  <si>
+    <t>real gemeinsam</t>
+  </si>
+  <si>
+    <t>real allein</t>
+  </si>
+  <si>
+    <t>acht/neun Jahre</t>
+  </si>
+  <si>
+    <t>sechs</t>
+  </si>
+  <si>
+    <t>unter drei</t>
+  </si>
+  <si>
+    <t>fünf/sechs</t>
+  </si>
+  <si>
+    <t>zehn und älter</t>
   </si>
 </sst>
 </file>
@@ -15482,9 +15515,9 @@
   <dimension ref="A1:BT210"/>
   <sheetViews>
     <sheetView topLeftCell="M2" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G2" sqref="G2"/>
-      <selection pane="bottomLeft" activeCell="AG2" sqref="AG2"/>
+      <selection pane="bottomLeft" activeCell="T100" sqref="T100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15496,7 +15529,9 @@
     <col min="10" max="10" width="13.6328125" customWidth="1"/>
     <col min="11" max="11" width="15.453125" customWidth="1"/>
     <col min="12" max="12" width="13.6328125" customWidth="1"/>
-    <col min="13" max="21" width="10.90625" customWidth="1"/>
+    <col min="13" max="15" width="10.90625" customWidth="1"/>
+    <col min="16" max="16" width="19" customWidth="1"/>
+    <col min="17" max="21" width="10.90625" customWidth="1"/>
     <col min="22" max="22" width="10.7265625" customWidth="1"/>
     <col min="23" max="23" width="13.6328125" customWidth="1"/>
     <col min="24" max="24" width="16.81640625" customWidth="1"/>
@@ -25212,6 +25247,12 @@
       </c>
     </row>
     <row r="89" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="Q89" t="s">
+        <v>533</v>
+      </c>
+      <c r="S89" t="s">
+        <v>532</v>
+      </c>
       <c r="U89" s="5" t="s">
         <v>500</v>
       </c>
@@ -25265,12 +25306,21 @@
       </c>
     </row>
     <row r="90" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="P90" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>478</v>
+      </c>
+      <c r="S90" t="s">
+        <v>477</v>
+      </c>
       <c r="U90">
-        <f>COUNTIF(X12:X31,"unter drei Jahren")</f>
-        <v>0</v>
+        <f>COUNTIF(X12:X31,"unter drei Jahre")</f>
+        <v>1</v>
       </c>
       <c r="V90">
-        <f>COUNTIF(X12:X31,"unter drei Jahren")</f>
+        <f>COUNTIF(Y12:Y31,"unter drei Jahren")</f>
         <v>0</v>
       </c>
       <c r="W90">
@@ -25325,9 +25375,18 @@
       </c>
     </row>
     <row r="91" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="P91" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>539</v>
+      </c>
+      <c r="S91" t="s">
+        <v>538</v>
+      </c>
       <c r="U91" s="6">
         <f>U90/W94</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="V91" s="6">
         <f>V90/W94</f>
@@ -25394,6 +25453,12 @@
       </c>
     </row>
     <row r="92" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="P92" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>540</v>
+      </c>
       <c r="U92" t="s">
         <v>479</v>
       </c>
@@ -25457,13 +25522,19 @@
       </c>
     </row>
     <row r="93" spans="1:72" x14ac:dyDescent="0.35">
+      <c r="P93" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>540</v>
+      </c>
       <c r="U93">
         <f>COUNTIF(X12:X31,"drei Jahre")</f>
         <v>1</v>
       </c>
       <c r="V93">
-        <f>COUNTIF(X12:X31,"drei Jahre")</f>
-        <v>1</v>
+        <f>COUNTIF(Y12:Y31,"drei Jahre")</f>
+        <v>0</v>
       </c>
       <c r="W93" t="s">
         <v>514</v>
@@ -25535,7 +25606,7 @@
       </c>
       <c r="V94" s="6">
         <f>V93/W94</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="W94" s="8">
         <f>COUNTA(X12:X31)</f>
@@ -25628,8 +25699,8 @@
         <v>2</v>
       </c>
       <c r="V96">
-        <f>COUNTIF(X12:X31,"vier Jahre")</f>
-        <v>2</v>
+        <f>COUNTIF(Y12:Y31,"vier Jahre")</f>
+        <v>0</v>
       </c>
       <c r="X96">
         <f>COUNTIF(X3:X10,"vier Jahre")</f>
@@ -25686,7 +25757,7 @@
       </c>
       <c r="V97" s="6">
         <f>V96/W94</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="X97" s="6">
         <f>X96/W90</f>
@@ -25817,8 +25888,8 @@
         <v>9</v>
       </c>
       <c r="V99">
-        <f>COUNTIF(X12:X31,"fünf Jahre")</f>
-        <v>9</v>
+        <f>COUNTIF(Y12:Y31,"fünf Jahre")</f>
+        <v>2</v>
       </c>
       <c r="X99">
         <f>COUNTIF(X3:X10,"fünf Jahre")</f>
@@ -25887,7 +25958,7 @@
       </c>
       <c r="V100" s="6">
         <f>V99/W94</f>
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="X100" s="6">
         <f>X99/W90</f>
@@ -25976,8 +26047,8 @@
         <v>3</v>
       </c>
       <c r="V102">
-        <f>COUNTIF(X12:X31,"sechs Jahre")</f>
-        <v>3</v>
+        <f>COUNTIF(Y12:Y31,"sechs Jahre")</f>
+        <v>2</v>
       </c>
       <c r="X102">
         <f>COUNTIF(X3:X10,"sechs Jahre")</f>
@@ -26034,7 +26105,7 @@
       </c>
       <c r="V103" s="6">
         <f>V102/W94</f>
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="X103" s="6">
         <f>X102/W90</f>
@@ -26165,8 +26236,8 @@
         <v>2</v>
       </c>
       <c r="V105">
-        <f>COUNTIF(X12:X31,"sieben Jahre")</f>
-        <v>2</v>
+        <f>COUNTIF(Y12:Y31,"sieben Jahre")</f>
+        <v>3</v>
       </c>
       <c r="X105">
         <f>COUNTIF(X3:X10,"sieben Jahre")</f>
@@ -26235,7 +26306,7 @@
       </c>
       <c r="V106" s="6">
         <f>V105/W94</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="X106" s="6">
         <f>X105/W90</f>
@@ -26324,8 +26395,8 @@
         <v>2</v>
       </c>
       <c r="V108">
-        <f>COUNTIF(X12:X31,"acht Jahre")</f>
-        <v>2</v>
+        <f>COUNTIF(Y12:Y31,"acht Jahre")</f>
+        <v>3</v>
       </c>
       <c r="X108">
         <f>COUNTIF(X3:X10,"acht Jahre")</f>
@@ -26382,7 +26453,7 @@
       </c>
       <c r="V109" s="6">
         <f>V108/W94</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="X109" s="6">
         <f>X108/W90</f>
@@ -26513,8 +26584,8 @@
         <v>0</v>
       </c>
       <c r="V111">
-        <f>COUNTIF(X12:X31,"neun Jahre")</f>
-        <v>0</v>
+        <f>COUNTIF(Y12:Y31,"neun Jahre")</f>
+        <v>2</v>
       </c>
       <c r="X111">
         <f>COUNTIF(X3:X10,"neun Jahre")</f>
@@ -26583,7 +26654,7 @@
       </c>
       <c r="V112" s="6">
         <f>V111/W94</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="X112" s="6">
         <f>X111/W90</f>
@@ -26645,7 +26716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="113" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U113" t="s">
         <v>484</v>
       </c>
@@ -26666,14 +26737,14 @@
       </c>
       <c r="AB113" s="10"/>
     </row>
-    <row r="114" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="114" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U114">
         <f>COUNTIF(X12:X31,"zehn Jahre und älter")</f>
         <v>0</v>
       </c>
       <c r="V114">
-        <f>COUNTIF(X12:X31,"zehn Jahre und älter")</f>
-        <v>0</v>
+        <f>COUNTIF(Y12:Y31,"zehn Jahre und älter")</f>
+        <v>8</v>
       </c>
       <c r="X114">
         <f>COUNTIF(X3:X10,"zehn Jahre und älter")</f>
@@ -26723,14 +26794,14 @@
         <v>505</v>
       </c>
     </row>
-    <row r="115" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="115" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U115" s="6">
         <f>U114/W94</f>
         <v>0</v>
       </c>
       <c r="V115" s="6">
         <f>V114/W94</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="X115" s="6">
         <f>X114/W90</f>
@@ -26792,14 +26863,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="116" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U116">
         <f>SUM(U114,U111,U108,U105,U102,U90,U93,U96,U99)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V116">
         <f>SUM(V90,V93,V96,V99,V102,V105,V108,V111,V114)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="X116">
         <f>SUM(X114,X111,X108,X105,X102,X90,X93,X96,X99)</f>
@@ -26861,14 +26932,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="117" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U117" s="6">
         <f>SUM(U115,U112,U109,U106,U103,U100,U97,U94,U91)</f>
-        <v>0.95000000000000007</v>
+        <v>1</v>
       </c>
       <c r="V117" s="6">
         <f>SUM(V115,V112,V109,V106,V103,V100,V97,V94,V91)</f>
-        <v>0.95000000000000007</v>
+        <v>1</v>
       </c>
       <c r="X117" s="6">
         <f>SUM(X115,X112,X109,X106,X103,X100,X97,X94,X91)</f>
@@ -26890,47 +26961,47 @@
         <v>516</v>
       </c>
       <c r="AC117">
-        <f>COUNTIF(AC12:AC31,"Sehr passend [4]")</f>
+        <f t="shared" ref="AC117:AL117" si="15">COUNTIF(AC12:AC31,"Sehr passend [4]")</f>
         <v>11</v>
       </c>
       <c r="AD117">
-        <f>COUNTIF(AD12:AD31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AE117">
-        <f>COUNTIF(AE12:AE31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="AF117">
-        <f>COUNTIF(AF12:AF31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="AG117">
-        <f>COUNTIF(AG12:AG31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AH117">
-        <f>COUNTIF(AH12:AH31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AI117">
-        <f>COUNTIF(AI12:AI31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AJ117">
-        <f>COUNTIF(AJ12:AJ31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AK117">
-        <f>COUNTIF(AK12:AK31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AL117">
-        <f>COUNTIF(AL12:AL31,"Sehr passend [4]")</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="118" spans="16:38" x14ac:dyDescent="0.35">
       <c r="AB118" s="10" t="s">
         <v>531</v>
       </c>
@@ -26975,13 +27046,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="119" spans="16:38" x14ac:dyDescent="0.35">
       <c r="W119" t="s">
         <v>510</v>
       </c>
       <c r="AB119" s="10"/>
     </row>
-    <row r="120" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="120" spans="16:38" x14ac:dyDescent="0.35">
+      <c r="Q120" t="s">
+        <v>533</v>
+      </c>
+      <c r="S120" t="s">
+        <v>532</v>
+      </c>
       <c r="U120" s="5" t="s">
         <v>500</v>
       </c>
@@ -27035,13 +27112,22 @@
         <v>527</v>
       </c>
     </row>
-    <row r="121" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="121" spans="16:38" x14ac:dyDescent="0.35">
+      <c r="P121" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>477</v>
+      </c>
+      <c r="S121" t="s">
+        <v>541</v>
+      </c>
       <c r="U121">
         <f>COUNTIF(X55:X60,"unter drei Jahren")</f>
         <v>0</v>
       </c>
       <c r="V121">
-        <f>COUNTIF(X55:X60,"unter drei Jahren")</f>
+        <f>COUNTIF(Y55:Y60,"unter drei Jahren")</f>
         <v>0</v>
       </c>
       <c r="W121">
@@ -27108,7 +27194,16 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="122" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="122" spans="16:38" x14ac:dyDescent="0.35">
+      <c r="P122" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>483</v>
+      </c>
+      <c r="S122" t="s">
+        <v>542</v>
+      </c>
       <c r="U122" s="6">
         <f>U121/W125</f>
         <v>0</v>
@@ -27134,7 +27229,13 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="123" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="123" spans="16:38" x14ac:dyDescent="0.35">
+      <c r="P123" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>477</v>
+      </c>
       <c r="U123" t="s">
         <v>479</v>
       </c>
@@ -27197,13 +27298,19 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="124" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="124" spans="16:38" x14ac:dyDescent="0.35">
+      <c r="P124" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>477</v>
+      </c>
       <c r="U124">
         <f>COUNTIF(X55:X60,"drei Jahre")</f>
         <v>0</v>
       </c>
       <c r="V124">
-        <f>COUNTIF(X55:X60,"drei Jahre")</f>
+        <f>COUNTIF(Y55:Y60,"drei Jahre")</f>
         <v>0</v>
       </c>
       <c r="W124" t="s">
@@ -27229,47 +27336,47 @@
         <v>529</v>
       </c>
       <c r="AC124">
-        <f>SUM(AC91,AC97,AC103,AC109,AC115)</f>
+        <f t="shared" ref="AC124:AL124" si="16">SUM(AC91,AC97,AC103,AC109,AC115)</f>
         <v>8</v>
       </c>
       <c r="AD124">
-        <f>SUM(AD91,AD97,AD103,AD109,AD115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AE124">
-        <f>SUM(AE91,AE97,AE103,AE109,AE115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AF124">
-        <f>SUM(AF91,AF97,AF103,AF109,AF115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AG124">
-        <f>SUM(AG91,AG97,AG103,AG109,AG115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AH124">
-        <f>SUM(AH91,AH97,AH103,AH109,AH115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AI124">
-        <f>SUM(AI91,AI97,AI103,AI109,AI115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AJ124">
-        <f>SUM(AJ91,AJ97,AJ103,AJ109,AJ115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AK124">
-        <f>SUM(AK91,AK97,AK103,AK109,AK115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="AL124">
-        <f>SUM(AL91,AL97,AL103,AL109,AL115)</f>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="125" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U125" s="6">
         <f>U124/W125</f>
         <v>0</v>
@@ -27302,47 +27409,47 @@
         <v>530</v>
       </c>
       <c r="AC125">
-        <f>SUM(AC93,AC99,AC105,AC111,AC117)</f>
+        <f t="shared" ref="AC125:AL125" si="17">SUM(AC93,AC99,AC105,AC111,AC117)</f>
         <v>20</v>
       </c>
       <c r="AD125">
-        <f>SUM(AD93,AD99,AD105,AD111,AD117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AE125">
-        <f>SUM(AE93,AE99,AE105,AE111,AE117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AF125">
-        <f>SUM(AF93,AF99,AF105,AF111,AF117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AG125">
-        <f>SUM(AG93,AG99,AG105,AG111,AG117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AH125">
-        <f>SUM(AH93,AH99,AH105,AH111,AH117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AI125">
-        <f>SUM(AI93,AI99,AI105,AI111,AI117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AJ125">
-        <f>SUM(AJ93,AJ99,AJ105,AJ111,AJ117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AK125">
-        <f>SUM(AK93,AK99,AK105,AK111,AK117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="AL125">
-        <f>SUM(AL93,AL99,AL105,AL111,AL117)</f>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="126" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U126" t="s">
         <v>478</v>
       </c>
@@ -27362,14 +27469,14 @@
         <v>478</v>
       </c>
     </row>
-    <row r="127" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="127" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U127">
         <f>COUNTIF(X55:X60,"vier Jahre")</f>
         <v>1</v>
       </c>
       <c r="V127">
-        <f>COUNTIF(X55:X60,"vier Jahre")</f>
-        <v>1</v>
+        <f>COUNTIF(Y55:Y60,"vier Jahre")</f>
+        <v>0</v>
       </c>
       <c r="X127">
         <f>COUNTIF(X33:X53,"vier Jahre")</f>
@@ -27388,14 +27495,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="21:38" x14ac:dyDescent="0.35">
+    <row r="128" spans="16:38" x14ac:dyDescent="0.35">
       <c r="U128" s="6">
         <f>U127/W125</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="V128" s="6">
         <f>V127/W125</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
       </c>
       <c r="X128" s="6">
         <f>X127/W121</f>
@@ -27471,39 +27578,39 @@
         <v>2</v>
       </c>
       <c r="AD129">
-        <f t="shared" ref="AD129:AL129" si="15">COUNTIF(AD33:AD53,"Absolut unpassend [0]")</f>
+        <f t="shared" ref="AD129:AL129" si="18">COUNTIF(AD33:AD53,"Absolut unpassend [0]")</f>
         <v>6</v>
       </c>
       <c r="AE129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="AF129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="AG129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="AH129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AI129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="AJ129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="AK129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="AL129">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
     </row>
@@ -27513,8 +27620,8 @@
         <v>2</v>
       </c>
       <c r="V130">
-        <f>COUNTIF(X55:X60,"fünf Jahre")</f>
-        <v>2</v>
+        <f>COUNTIF(Y55:Y60,"fünf Jahre")</f>
+        <v>0</v>
       </c>
       <c r="X130">
         <f>COUNTIF(X33:X53,"fünf Jahre")</f>
@@ -27583,7 +27690,7 @@
       </c>
       <c r="V131" s="6">
         <f>V130/W125</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="X131" s="6">
         <f>X130/W121</f>
@@ -27609,39 +27716,39 @@
         <v>0</v>
       </c>
       <c r="AD131">
-        <f t="shared" ref="AD131:AL131" si="16">COUNTIF(AD55:AD60,"Absolut unpassend [0]")</f>
+        <f t="shared" ref="AD131:AL131" si="19">COUNTIF(AD55:AD60,"Absolut unpassend [0]")</f>
         <v>0</v>
       </c>
       <c r="AE131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AF131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AG131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="AH131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="AI131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
       <c r="AJ131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5</v>
       </c>
       <c r="AK131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="AL131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -27714,8 +27821,8 @@
         <v>1</v>
       </c>
       <c r="V133">
-        <f>COUNTIF(X55:X60,"sechs Jahre")</f>
-        <v>1</v>
+        <f>COUNTIF(Y55:Y60,"sechs Jahre")</f>
+        <v>0</v>
       </c>
       <c r="X133">
         <f>COUNTIF(X33:X53,"sechs Jahre")</f>
@@ -27742,7 +27849,7 @@
       </c>
       <c r="V134" s="6">
         <f>V133/W125</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
       </c>
       <c r="X134" s="6">
         <f>X133/W121</f>
@@ -27819,39 +27926,39 @@
         <v>1</v>
       </c>
       <c r="AD135">
-        <f t="shared" ref="AD135:AL135" si="17">COUNTIF(AD33:AD53,"Eher unpassend [1]")</f>
+        <f t="shared" ref="AD135:AL135" si="20">COUNTIF(AD33:AD53,"Eher unpassend [1]")</f>
         <v>0</v>
       </c>
       <c r="AE135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AF135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AG135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="AH135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="AI135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="AJ135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="AK135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
       <c r="AL135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
     </row>
@@ -27861,7 +27968,7 @@
         <v>0</v>
       </c>
       <c r="V136">
-        <f>COUNTIF(X55:X60,"sieben Jahre")</f>
+        <f>COUNTIF(Y55:Y60,"sieben Jahre")</f>
         <v>0</v>
       </c>
       <c r="X136">
@@ -27957,39 +28064,39 @@
         <v>1</v>
       </c>
       <c r="AD137">
-        <f t="shared" ref="AD137:AL137" si="18">COUNTIF(AD55:AD60,"Eher unpassend [1]")</f>
+        <f t="shared" ref="AD137:AL137" si="21">COUNTIF(AD55:AD60,"Eher unpassend [1]")</f>
         <v>2</v>
       </c>
       <c r="AE137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AF137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AG137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="AH137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AI137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AJ137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AK137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="AL137">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
@@ -28062,8 +28169,8 @@
         <v>1</v>
       </c>
       <c r="V139">
-        <f>COUNTIF(X55:X60,"acht Jahre")</f>
-        <v>1</v>
+        <f>COUNTIF(Y55:Y60,"acht Jahre")</f>
+        <v>0</v>
       </c>
       <c r="X139">
         <f>COUNTIF(X33:X53,"acht Jahre")</f>
@@ -28090,7 +28197,7 @@
       </c>
       <c r="V140" s="6">
         <f>V139/W125</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
       </c>
       <c r="X140" s="6">
         <f>X139/W121</f>
@@ -28167,39 +28274,39 @@
         <v>2</v>
       </c>
       <c r="AD141">
-        <f t="shared" ref="AD141:AL141" si="19">COUNTIF(AD33:AD53,"neutral [2]")</f>
+        <f t="shared" ref="AD141:AL141" si="22">COUNTIF(AD33:AD53,"neutral [2]")</f>
         <v>5</v>
       </c>
       <c r="AE141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="AF141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="AG141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="AH141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="AI141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="AJ141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="AK141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="AL141">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
     </row>
@@ -28209,8 +28316,8 @@
         <v>0</v>
       </c>
       <c r="V142">
-        <f>COUNTIF(X55:X60,"neun Jahre")</f>
-        <v>0</v>
+        <f>COUNTIF(Y55:Y60,"neun Jahre")</f>
+        <v>1</v>
       </c>
       <c r="X142">
         <f>COUNTIF(X33:X53,"neun Jahre")</f>
@@ -28279,7 +28386,7 @@
       </c>
       <c r="V143" s="6">
         <f>V142/W125</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="X143" s="6">
         <f>X142/W121</f>
@@ -28305,39 +28412,39 @@
         <v>1</v>
       </c>
       <c r="AD143">
-        <f t="shared" ref="AD143:AL143" si="20">COUNTIF(AD55:AD60,"neutral [2]")</f>
+        <f t="shared" ref="AD143:AL143" si="23">COUNTIF(AD55:AD60,"neutral [2]")</f>
         <v>1</v>
       </c>
       <c r="AE143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="AF143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="AG143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="AH143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="AI143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="AJ143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="AK143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="AL143">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
     </row>
@@ -28410,8 +28517,8 @@
         <v>1</v>
       </c>
       <c r="V145">
-        <f>COUNTIF(X55:X60,"zehn Jahre und älter")</f>
-        <v>1</v>
+        <f>COUNTIF(Y55:Y60,"zehn Jahre und älter")</f>
+        <v>5</v>
       </c>
       <c r="X145">
         <f>COUNTIF(X33:X53,"zehn Jahre und älter")</f>
@@ -28438,7 +28545,7 @@
       </c>
       <c r="V146" s="6">
         <f>V145/W125</f>
-        <v>0.16666666666666666</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="X146" s="6">
         <f>X145/W121</f>
@@ -28521,39 +28628,39 @@
         <v>2</v>
       </c>
       <c r="AD147">
-        <f t="shared" ref="AD147:AL147" si="21">COUNTIF(AD33:AD53,"eher passend [3]")</f>
+        <f t="shared" ref="AD147:AL147" si="24">COUNTIF(AD33:AD53,"eher passend [3]")</f>
         <v>5</v>
       </c>
       <c r="AE147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
       <c r="AF147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>5</v>
       </c>
       <c r="AG147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="AH147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="AI147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="AJ147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="AK147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="AL147">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
     </row>
@@ -28564,7 +28671,7 @@
       </c>
       <c r="V148" s="6">
         <f>SUM(V146,V143,V140,V137,V134,V131,V128,V125,V122)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="X148" s="6">
         <f>SUM(X146,X143,X140,X137,X134,X131,X128,X125,X122)</f>
@@ -28635,39 +28742,39 @@
         <v>1</v>
       </c>
       <c r="AD149">
-        <f t="shared" ref="AD149:AL149" si="22">COUNTIF(AD55:AD60,"eher passend [3]")</f>
+        <f t="shared" ref="AD149:AL149" si="25">COUNTIF(AD55:AD60,"eher passend [3]")</f>
         <v>2</v>
       </c>
       <c r="AE149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="AF149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="AG149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AH149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AI149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AJ149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AK149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AL149">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -28837,39 +28944,39 @@
         <v>14</v>
       </c>
       <c r="AD153">
-        <f t="shared" ref="AD153:AL153" si="23">COUNTIF(AD33:AD53,"Sehr passend [4]")</f>
+        <f t="shared" ref="AD153:AL153" si="26">COUNTIF(AD33:AD53,"Sehr passend [4]")</f>
         <v>5</v>
       </c>
       <c r="AE153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>5</v>
       </c>
       <c r="AF153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>12</v>
       </c>
       <c r="AG153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="AH153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="AI153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AJ153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="AK153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="AL153">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
@@ -28976,35 +29083,35 @@
         <v>1</v>
       </c>
       <c r="AE155">
-        <f t="shared" ref="AD155:AL155" si="24">COUNTIF(AE55:AE60,"Sehr passend [4]")</f>
+        <f t="shared" ref="AE155:AL155" si="27">COUNTIF(AE55:AE60,"Sehr passend [4]")</f>
         <v>2</v>
       </c>
       <c r="AF155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="AG155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="AH155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AI155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AJ155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AK155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AL155">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -29346,43 +29453,43 @@
         <v>529</v>
       </c>
       <c r="AC162">
-        <f>SUM(AC129,AC135,AC141,AC147,AC153)</f>
+        <f t="shared" ref="AC162:AL162" si="28">SUM(AC129,AC135,AC141,AC147,AC153)</f>
         <v>21</v>
       </c>
       <c r="AD162">
-        <f>SUM(AD129,AD135,AD141,AD147,AD153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AE162">
-        <f>SUM(AE129,AE135,AE141,AE147,AE153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AF162">
-        <f>SUM(AF129,AF135,AF141,AF147,AF153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AG162">
-        <f>SUM(AG129,AG135,AG141,AG147,AG153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AH162">
-        <f>SUM(AH129,AH135,AH141,AH147,AH153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AI162">
-        <f>SUM(AI129,AI135,AI141,AI147,AI153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AJ162">
-        <f>SUM(AJ129,AJ135,AJ141,AJ147,AJ153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AK162">
-        <f>SUM(AK129,AK135,AK141,AK147,AK153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
       <c r="AL162">
-        <f>SUM(AL129,AL135,AL141,AL147,AL153)</f>
+        <f t="shared" si="28"/>
         <v>21</v>
       </c>
     </row>
@@ -29409,43 +29516,43 @@
         <v>530</v>
       </c>
       <c r="AC163">
-        <f>SUM(AC131,AC137,AC143,AC149,AC155)</f>
+        <f t="shared" ref="AC163:AL163" si="29">SUM(AC131,AC137,AC143,AC149,AC155)</f>
         <v>6</v>
       </c>
       <c r="AD163">
-        <f>SUM(AD131,AD137,AD143,AD149,AD155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AE163">
-        <f>SUM(AE131,AE137,AE143,AE149,AE155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AF163">
-        <f>SUM(AF131,AF137,AF143,AF149,AF155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AG163">
-        <f>SUM(AG131,AG137,AG143,AG149,AG155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AH163">
-        <f>SUM(AH131,AH137,AH143,AH149,AH155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AI163">
-        <f>SUM(AI131,AI137,AI143,AI149,AI155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AJ163">
-        <f>SUM(AJ131,AJ137,AJ143,AJ149,AJ155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AK163">
-        <f>SUM(AK131,AK137,AK143,AK149,AK155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="AL163">
-        <f>SUM(AL131,AL137,AL143,AL149,AL155)</f>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
     </row>
@@ -30348,7 +30455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F38EF43-BB35-4395-A9FF-1EA0BCAD0259}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>

</xml_diff>